<commit_message>
inserted mapping values #492
</commit_message>
<xml_diff>
--- a/import/raw_data/mapping__parameter__start_year_usage.xlsx
+++ b/import/raw_data/mapping__parameter__start_year_usage.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_env\workspace\micat\import\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D084B0-5916-4F2C-9EFC-6AED6B8B3BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B6B584-EE7F-4A8A-AE30-591816577AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="3180" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="1560" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="id_indicator_group_mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -350,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:C65"/>
+      <selection activeCell="C2" sqref="C2:C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +427,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -425,7 +438,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -436,7 +449,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -447,7 +460,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,7 +471,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -469,7 +482,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,7 +537,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,7 +548,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -557,7 +570,7 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,7 +581,7 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,7 +636,7 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -645,7 +658,7 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -656,7 +669,7 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -722,7 +735,7 @@
         <v>32</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,7 +757,7 @@
         <v>34</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,7 +768,7 @@
         <v>35</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -788,7 +801,7 @@
         <v>38</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -799,7 +812,7 @@
         <v>39</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -810,7 +823,7 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -821,7 +834,7 @@
         <v>41</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -843,7 +856,7 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -865,7 +878,7 @@
         <v>45</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -898,7 +911,7 @@
         <v>48</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,7 +933,7 @@
         <v>50</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -953,7 +966,7 @@
         <v>53</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,7 +977,7 @@
         <v>54</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -975,7 +988,7 @@
         <v>55</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,17 +1076,6 @@
         <v>63</v>
       </c>
       <c r="C64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>64</v>
-      </c>
-      <c r="C65">
         <v>1</v>
       </c>
     </row>

</xml_diff>